<commit_message>
Study part 1 + fixed part 2
</commit_message>
<xml_diff>
--- a/Zadanie 2 - Sprawozdanie/Wyniki.xlsx
+++ b/Zadanie 2 - Sprawozdanie/Wyniki.xlsx
@@ -4,18 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9552" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="2.1" sheetId="1" r:id="rId1"/>
-    <sheet name="2.2" sheetId="2" r:id="rId2"/>
+    <sheet name="_xltb_storage_" sheetId="3" state="veryHidden" r:id="rId1"/>
+    <sheet name="1.1" sheetId="4" r:id="rId2"/>
+    <sheet name="1.2" sheetId="5" r:id="rId3"/>
+    <sheet name="1.3" sheetId="6" r:id="rId4"/>
+    <sheet name="2.1" sheetId="1" r:id="rId5"/>
+    <sheet name="2.2" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="116">
   <si>
     <t>Żaden piłkarzy posiadających/będących Słaby Balans mają/są Przeciętne Reakcje</t>
   </si>
@@ -240,6 +244,138 @@
   </si>
   <si>
     <t>Standardowa waga</t>
+  </si>
+  <si>
+    <t>XL Toolbox Settings</t>
+  </si>
+  <si>
+    <t>export_preset</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="utf-16"?&gt;_x000D_
+&lt;Preset xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance"&gt;_x000D_
+  &lt;Name&gt;Png, 600 dpi, RGB, Transparent canvas&lt;/Name&gt;_x000D_
+  &lt;Dpi&gt;600&lt;/Dpi&gt;_x000D_
+  &lt;FileType&gt;Png&lt;/FileType&gt;_x000D_
+  &lt;ColorSpace&gt;Rgb&lt;/ColorSpace&gt;_x000D_
+  &lt;Transparency&gt;TransparentCanvas&lt;/Transparency&gt;_x000D_
+  &lt;UseColorProfile&gt;false&lt;/UseColorProfile&gt;_x000D_
+  &lt;ColorProfile&gt;ProPhoto&lt;/ColorProfile&gt;_x000D_
+&lt;/Preset&gt;</t>
+  </si>
+  <si>
+    <t>export_path</t>
+  </si>
+  <si>
+    <t>D:\Nauka\Git\KSR\Zadanie 2 - Sprawozdanie\Rysunki\Badanie2.2.2.png</t>
+  </si>
+  <si>
+    <t>Żaden piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Mniej niż ćwierć piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Około jedna trzecia piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Około połowa piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Około dwie trzecie piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Większość piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Prawie każdy piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Mniej niż 100 piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Około 250 piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Około 500 piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Około 750 piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Więcej niż 1000 piłkarzy posiadających/będących Dobra Celność mają/są Przeciętne Ustawianie się</t>
+  </si>
+  <si>
+    <t>Żaden piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Mniej niż ćwierć piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Około jedna trzecia piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Około połowa piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Około dwie trzecie piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Większość piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Prawie każdy piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Mniej niż 100 piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Około 250 piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Około 500 piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Około 750 piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Więcej niż 1000 piłkarzy posiadających/będących Dobry Dribbling mają/są Przeciętne Przyspieszenie</t>
+  </si>
+  <si>
+    <t>Żaden piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
+  </si>
+  <si>
+    <t>Mniej niż ćwierć piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
+  </si>
+  <si>
+    <t>Około jedna trzecia piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
+  </si>
+  <si>
+    <t>Około połowa piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
+  </si>
+  <si>
+    <t>Około dwie trzecie piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
+  </si>
+  <si>
+    <t>Większość piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
+  </si>
+  <si>
+    <t>Prawie każdy piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
+  </si>
+  <si>
+    <t>Mniej niż 100 piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
+  </si>
+  <si>
+    <t>Około 250 piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
+  </si>
+  <si>
+    <t>Około 500 piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
+  </si>
+  <si>
+    <t>Około 750 piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
+  </si>
+  <si>
+    <t>Więcej niż 1000 piłkarzy posiadających/będących Młody Wiek mają/są Postawna Waga</t>
   </si>
 </sst>
 </file>
@@ -742,9 +878,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -829,6 +969,523 @@
               <a:rPr lang="pl-PL" sz="1400">
                 <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
               </a:rPr>
+              <a:t>X piłkarzy posiadajcych dobrą celność ma Przeciętne Ustawianie</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400" baseline="0">
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:rPr>
+              <a:t> się</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1.1'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>'1.1'!$C$2:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.46800000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1.1'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="002060"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'1.1'!$B$2:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Żaden</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mniej niż 1/4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Około 1/3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Około 1/2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Około 2/3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Większość</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Prawie każdy</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Mniej niż 100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Około 250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Około 500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Około 750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Więcej niż 1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1.1'!$H$2:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.98699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.2E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1.1'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>T7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'1.1'!$B$2:$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Żaden</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mniej niż 1/4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Około 1/3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Około 1/2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Około 2/3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Większość</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Prawie każdy</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Mniej niż 100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Około 250</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Około 500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Około 750</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Więcej niż 1000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1.1'!$I$2:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="674494976"/>
+        <c:axId val="145639680"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="674494976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Miara podsumowania</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="900">
+                  <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="145639680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="145639680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:rPr>
+                  <a:t>Wartość miary</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="674494976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400">
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400">
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:rPr>
               <a:t>Około 2/3 piłkarzy ma Przeciętne Reakcje</a:t>
             </a:r>
           </a:p>
@@ -925,7 +1582,7 @@
                   <c:v>0.77600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.77600000000000002</c:v>
+                  <c:v>0.16300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -1044,7 +1701,7 @@
                   <c:v>0.80600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.80600000000000005</c:v>
+                  <c:v>0.192</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -1092,6 +1749,32 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Miara podsumowania</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="900">
+                  <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1123,6 +1806,29 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:rPr>
+                  <a:t>Wartość miary</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1173,7 +1879,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pl-PL"/>
@@ -1298,7 +2004,7 @@
                   <c:v>0.77600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.77600000000000002</c:v>
+                  <c:v>0.16300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -1417,7 +2123,7 @@
                   <c:v>0.80600000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.80600000000000005</c:v>
+                  <c:v>0.192</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -1465,6 +2171,32 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Miara podsumowania</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="900">
+                  <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1496,6 +2228,29 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:rPr>
+                  <a:t>Wartość miary</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -1513,498 +2268,6 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="139435008"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr>
-              <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400">
-                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pl-PL" sz="1400">
-                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
-              </a:rPr>
-              <a:t>X piłkarzy ma Standardową</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pl-PL" sz="1400" baseline="0">
-                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
-              </a:rPr>
-              <a:t> Wagę</a:t>
-            </a:r>
-            <a:endParaRPr lang="pl-PL" sz="1400">
-              <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Mniej niż 1/4 - Niski wzrost</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="002060"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:srgbClr val="002060"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2.2'!$C$1:$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>T1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>T2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>T3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>T4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>T5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>T6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>T7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>T8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>T9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>T10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>T11</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2.2'!$C$3:$M$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.48199999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.8000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.8000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.96599999999999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Mniej niż 1/4 - brak kwalifikatora</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2.2'!$C$1:$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>T1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>T2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>T3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>T4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>T5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>T6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>T7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>T8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>T9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>T10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>T11</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2.2'!$C$17:$M$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>9.4E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.48199999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.51800000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.51800000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.65</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.99399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Około 1/3 - brak kwalifikatora</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent5">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'2.2'!$C$1:$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>T1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>T2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>T3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>T4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>T5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>T6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>T7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>T8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>T9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>T10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>T11</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'2.2'!$C$18:$M$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0.89400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.48199999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.51800000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.51800000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.99399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="158572032"/>
-        <c:axId val="593320704"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="158572032"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr>
-                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="593320704"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="593320704"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr>
-                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="158572032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2094,6 +2357,544 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
+            <c:v>Mniej niż 1/4 - Niski wzrost</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="002060"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2.2'!$C$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>T2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>T3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>T4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>T5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>T6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>T7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>T8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>T11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2.2'!$C$3:$M$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.96599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mniej niż 1/4 - brak kwalifikatora</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2.2'!$C$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>T2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>T3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>T4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>T5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>T6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>T7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>T8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>T11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2.2'!$C$17:$M$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>9.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Około 1/3 - brak kwalifikatora</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2.2'!$C$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>T2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>T3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>T4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>T5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>T6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>T7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>T8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>T9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>T10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>T11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2.2'!$C$18:$M$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.89400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.48199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.51800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="158572032"/>
+        <c:axId val="593320704"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="158572032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:rPr>
+                  <a:t>Miara podsumowania</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="593320704"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="593320704"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:rPr>
+                  <a:t>Wartość miary</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr>
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pl-PL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="158572032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr>
+              <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pl-PL"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400">
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400">
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:rPr>
+              <a:t>X piłkarzy ma Standardową</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pl-PL" sz="1400" baseline="0">
+                <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+              </a:rPr>
+              <a:t> Wagę</a:t>
+            </a:r>
+            <a:endParaRPr lang="pl-PL" sz="1400">
+              <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
             <c:v>Mniej niż 100 - Niski wzrost</c:v>
           </c:tx>
           <c:spPr>
@@ -2172,7 +2973,7 @@
                   <c:v>4.8000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.8000000000000001E-2</c:v>
+                  <c:v>0.29299999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -2291,7 +3092,7 @@
                   <c:v>0.51800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.51800000000000002</c:v>
+                  <c:v>0.17799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
@@ -2339,6 +3140,31 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:rPr>
+                  <a:t>Miara podsumowania</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL" sz="900">
+                  <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2370,6 +3196,29 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL" sz="900">
+                    <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
+                  </a:rPr>
+                  <a:t>Wartość miary</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -2421,6 +3270,43 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5781000</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>24720</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Wykres 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2487,7 +3373,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2843,10 +3729,1684 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="87.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="D2">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E2">
+        <v>0.151</v>
+      </c>
+      <c r="F2">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.9</v>
+      </c>
+      <c r="I2">
+        <v>0.95</v>
+      </c>
+      <c r="J2">
+        <v>0.998</v>
+      </c>
+      <c r="K2">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L2">
+        <v>0.999</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.151</v>
+      </c>
+      <c r="F3">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.65</v>
+      </c>
+      <c r="I3">
+        <v>0.7</v>
+      </c>
+      <c r="J3">
+        <v>0.998</v>
+      </c>
+      <c r="K3">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L3">
+        <v>0.999</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.151</v>
+      </c>
+      <c r="F4">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.8</v>
+      </c>
+      <c r="I4">
+        <v>0.9</v>
+      </c>
+      <c r="J4">
+        <v>0.998</v>
+      </c>
+      <c r="K4">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L4">
+        <v>0.999</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.151</v>
+      </c>
+      <c r="F5">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.8</v>
+      </c>
+      <c r="I5">
+        <v>0.9</v>
+      </c>
+      <c r="J5">
+        <v>0.998</v>
+      </c>
+      <c r="K5">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L5">
+        <v>0.999</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.151</v>
+      </c>
+      <c r="F6">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.8</v>
+      </c>
+      <c r="I6">
+        <v>0.9</v>
+      </c>
+      <c r="J6">
+        <v>0.998</v>
+      </c>
+      <c r="K6">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L6">
+        <v>0.999</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E7">
+        <v>0.151</v>
+      </c>
+      <c r="F7">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.8</v>
+      </c>
+      <c r="I7">
+        <v>0.9</v>
+      </c>
+      <c r="J7">
+        <v>0.998</v>
+      </c>
+      <c r="K7">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L7">
+        <v>0.999</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.151</v>
+      </c>
+      <c r="F8">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0.8</v>
+      </c>
+      <c r="I8">
+        <v>0.9</v>
+      </c>
+      <c r="J8">
+        <v>0.998</v>
+      </c>
+      <c r="K8">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L8">
+        <v>0.999</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E9">
+        <v>0.151</v>
+      </c>
+      <c r="F9">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.99</v>
+      </c>
+      <c r="I9">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="J9">
+        <v>0.998</v>
+      </c>
+      <c r="K9">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L9">
+        <v>0.999</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E10">
+        <v>0.151</v>
+      </c>
+      <c r="F10">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J10">
+        <v>0.998</v>
+      </c>
+      <c r="K10">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L10">
+        <v>0.999</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.151</v>
+      </c>
+      <c r="F11">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I11">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J11">
+        <v>0.998</v>
+      </c>
+      <c r="K11">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L11">
+        <v>0.999</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.151</v>
+      </c>
+      <c r="F12">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I12">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J12">
+        <v>0.998</v>
+      </c>
+      <c r="K12">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L12">
+        <v>0.999</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="E13">
+        <v>0.151</v>
+      </c>
+      <c r="F13">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I13">
+        <v>6.3E-2</v>
+      </c>
+      <c r="J13">
+        <v>0.998</v>
+      </c>
+      <c r="K13">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="L13">
+        <v>0.999</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="87" customWidth="1"/>
+    <col min="2" max="2" width="15.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E2">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F2">
+        <v>0.127</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.9</v>
+      </c>
+      <c r="I2">
+        <v>0.95</v>
+      </c>
+      <c r="J2">
+        <v>0.999</v>
+      </c>
+      <c r="K2">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L2">
+        <v>0.999</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E3">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.127</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.65</v>
+      </c>
+      <c r="I3">
+        <v>0.7</v>
+      </c>
+      <c r="J3">
+        <v>0.999</v>
+      </c>
+      <c r="K3">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L3">
+        <v>0.999</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E4">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.127</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.8</v>
+      </c>
+      <c r="I4">
+        <v>0.9</v>
+      </c>
+      <c r="J4">
+        <v>0.999</v>
+      </c>
+      <c r="K4">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L4">
+        <v>0.999</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.127</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.8</v>
+      </c>
+      <c r="I5">
+        <v>0.9</v>
+      </c>
+      <c r="J5">
+        <v>0.999</v>
+      </c>
+      <c r="K5">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L5">
+        <v>0.999</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.127</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.8</v>
+      </c>
+      <c r="I6">
+        <v>0.9</v>
+      </c>
+      <c r="J6">
+        <v>0.999</v>
+      </c>
+      <c r="K6">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L6">
+        <v>0.999</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E7">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.127</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.8</v>
+      </c>
+      <c r="I7">
+        <v>0.9</v>
+      </c>
+      <c r="J7">
+        <v>0.999</v>
+      </c>
+      <c r="K7">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L7">
+        <v>0.999</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.127</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0.8</v>
+      </c>
+      <c r="I8">
+        <v>0.9</v>
+      </c>
+      <c r="J8">
+        <v>0.999</v>
+      </c>
+      <c r="K8">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L8">
+        <v>0.999</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E9">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F9">
+        <v>0.127</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.99</v>
+      </c>
+      <c r="I9">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="J9">
+        <v>0.999</v>
+      </c>
+      <c r="K9">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L9">
+        <v>0.999</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10">
+        <v>0.189</v>
+      </c>
+      <c r="D10">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E10">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.127</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J10">
+        <v>0.999</v>
+      </c>
+      <c r="K10">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L10">
+        <v>0.999</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E11">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F11">
+        <v>0.127</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I11">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J11">
+        <v>0.999</v>
+      </c>
+      <c r="K11">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L11">
+        <v>0.999</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F12">
+        <v>0.127</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I12">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J12">
+        <v>0.999</v>
+      </c>
+      <c r="K12">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L12">
+        <v>0.999</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.61399999999999999</v>
+      </c>
+      <c r="E13">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="F13">
+        <v>0.127</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I13">
+        <v>6.3E-2</v>
+      </c>
+      <c r="J13">
+        <v>0.999</v>
+      </c>
+      <c r="K13">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="L13">
+        <v>0.999</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="79" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2">
+        <v>0.253</v>
+      </c>
+      <c r="D2">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F2">
+        <v>0.02</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0.9</v>
+      </c>
+      <c r="I2">
+        <v>0.95</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F3">
+        <v>0.02</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0.65</v>
+      </c>
+      <c r="I3">
+        <v>0.7</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.02</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0.8</v>
+      </c>
+      <c r="I4">
+        <v>0.9</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.02</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0.8</v>
+      </c>
+      <c r="I5">
+        <v>0.9</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F6">
+        <v>0.02</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>0.8</v>
+      </c>
+      <c r="I6">
+        <v>0.9</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F7">
+        <v>0.02</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.8</v>
+      </c>
+      <c r="I7">
+        <v>0.9</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E8">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F8">
+        <v>0.02</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0.8</v>
+      </c>
+      <c r="I8">
+        <v>0.9</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.02</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>0.99</v>
+      </c>
+      <c r="I9">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F10">
+        <v>0.02</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E11">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.02</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I11">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E12">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F12">
+        <v>0.02</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="I12">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0.88700000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="F13">
+        <v>0.02</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>6.2E-2</v>
+      </c>
+      <c r="I13">
+        <v>6.3E-2</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2910,7 +5470,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F2">
-        <v>0.77600000000000002</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2951,7 +5511,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F3">
-        <v>0.77600000000000002</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2992,7 +5552,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F4">
-        <v>0.77600000000000002</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -3033,7 +5593,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F5">
-        <v>0.77600000000000002</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -3074,7 +5634,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F6" s="1">
-        <v>0.77600000000000002</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G6" s="1">
         <v>1</v>
@@ -3115,7 +5675,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F7">
-        <v>0.77600000000000002</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -3156,7 +5716,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F8">
-        <v>0.77600000000000002</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3197,7 +5757,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F9">
-        <v>0.77600000000000002</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -3238,7 +5798,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F10">
-        <v>0.77600000000000002</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -3279,7 +5839,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F11" s="1">
-        <v>0.77600000000000002</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
@@ -3320,7 +5880,7 @@
         <v>0.77600000000000002</v>
       </c>
       <c r="F12">
-        <v>0.77600000000000002</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -3348,40 +5908,40 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1">
+      <c r="C13" s="3">
+        <v>0</v>
+      </c>
+      <c r="D13" s="3">
         <v>0.19400000000000001</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="3">
         <v>0.77600000000000002</v>
       </c>
-      <c r="F13" s="1">
-        <v>0.77600000000000002</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
+      <c r="F13" s="3">
+        <v>0.16300000000000001</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
         <v>6.2E-2</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="3">
         <v>6.3E-2</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="3">
         <v>0.999</v>
       </c>
-      <c r="K13" s="1">
+      <c r="K13" s="3">
         <v>0.92800000000000005</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="3">
         <v>0.999</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M13" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3407,7 +5967,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="F16">
-        <v>0.80600000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -3448,7 +6008,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="F17">
-        <v>0.80600000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -3489,7 +6049,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="F18">
-        <v>0.80600000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -3530,7 +6090,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="F19">
-        <v>0.80600000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -3571,7 +6131,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="F20" s="1">
-        <v>0.80600000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="G20" s="1">
         <v>1</v>
@@ -3612,7 +6172,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="F21">
-        <v>0.80600000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -3653,7 +6213,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="F22">
-        <v>0.80600000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -3694,7 +6254,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="F23">
-        <v>0.80600000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -3735,7 +6295,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="F24">
-        <v>0.80600000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -3763,40 +6323,40 @@
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="1">
-        <v>0</v>
-      </c>
-      <c r="D25" s="1">
+      <c r="C25" s="3">
+        <v>0</v>
+      </c>
+      <c r="D25" s="3">
         <v>0.19400000000000001</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="3">
         <v>0.80600000000000005</v>
       </c>
-      <c r="F25" s="1">
-        <v>0.80600000000000005</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="F25" s="3">
+        <v>0.192</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
         <v>0.98699999999999999</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="3">
         <v>0.99399999999999999</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="3">
         <v>0.999</v>
       </c>
-      <c r="K25" s="1">
-        <v>0</v>
-      </c>
-      <c r="L25" s="1">
+      <c r="K25" s="3">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3">
         <v>0.99399999999999999</v>
       </c>
-      <c r="M25" s="1">
+      <c r="M25" s="3">
         <v>1</v>
       </c>
     </row>
@@ -3817,7 +6377,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="F26">
-        <v>0.80600000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -3858,7 +6418,7 @@
         <v>0.80600000000000005</v>
       </c>
       <c r="F27" s="1">
-        <v>0.80600000000000005</v>
+        <v>0.192</v>
       </c>
       <c r="G27" s="1">
         <v>1</v>
@@ -3889,12 +6449,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3958,7 +6518,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F2">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -3999,7 +6559,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
@@ -4040,7 +6600,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F4">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -4081,7 +6641,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F5">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -4122,7 +6682,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F6">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -4163,7 +6723,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F7">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -4204,7 +6764,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F8">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -4245,7 +6805,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F9" s="1">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G9" s="1">
         <v>1</v>
@@ -4286,7 +6846,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F10">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -4327,7 +6887,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F11">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -4368,7 +6928,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F12">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -4409,7 +6969,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F13">
-        <v>4.8000000000000001E-2</v>
+        <v>0.29299999999999998</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -4455,7 +7015,7 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="F16">
-        <v>0.51800000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -4483,40 +7043,40 @@
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="3">
         <v>9.4E-2</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="3">
         <v>0.48199999999999998</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="3">
         <v>0.51800000000000002</v>
       </c>
-      <c r="F17" s="1">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1">
+      <c r="F17" s="3">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
         <v>0.65</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="3">
         <v>0.7</v>
       </c>
-      <c r="J17" s="1">
-        <v>1</v>
-      </c>
-      <c r="K17" s="1">
-        <v>0</v>
-      </c>
-      <c r="L17" s="1">
+      <c r="J17" s="3">
+        <v>1</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3">
         <v>0.99399999999999999</v>
       </c>
-      <c r="M17" s="1">
+      <c r="M17" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4524,40 +7084,40 @@
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="3">
         <v>0.89400000000000002</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="3">
         <v>0.48199999999999998</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="3">
         <v>0.51800000000000002</v>
       </c>
-      <c r="F18" s="1">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1">
+      <c r="F18" s="3">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
         <v>0.8</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="3">
         <v>0.9</v>
       </c>
-      <c r="J18" s="1">
-        <v>1</v>
-      </c>
-      <c r="K18" s="1">
-        <v>0</v>
-      </c>
-      <c r="L18" s="1">
+      <c r="J18" s="3">
+        <v>1</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
         <v>0.99399999999999999</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M18" s="3">
         <v>1</v>
       </c>
     </row>
@@ -4578,7 +7138,7 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="F19">
-        <v>0.51800000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -4619,7 +7179,7 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="F20">
-        <v>0.51800000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -4660,7 +7220,7 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="F21">
-        <v>0.51800000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -4701,7 +7261,7 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="F22">
-        <v>0.51800000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -4742,7 +7302,7 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="F23">
-        <v>0.51800000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -4783,7 +7343,7 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="F24">
-        <v>0.51800000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -4824,7 +7384,7 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="F25">
-        <v>0.51800000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -4865,7 +7425,7 @@
         <v>0.51800000000000002</v>
       </c>
       <c r="F26">
-        <v>0.51800000000000002</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -4893,40 +7453,40 @@
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
         <v>0.48199999999999998</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="3">
         <v>0.51800000000000002</v>
       </c>
-      <c r="F27" s="1">
-        <v>0.51800000000000002</v>
-      </c>
-      <c r="G27" s="1">
-        <v>1</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="F27" s="3">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1</v>
+      </c>
+      <c r="H27" s="3">
         <v>6.2E-2</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="3">
         <v>6.3E-2</v>
       </c>
-      <c r="J27" s="1">
-        <v>1</v>
-      </c>
-      <c r="K27" s="1">
-        <v>0</v>
-      </c>
-      <c r="L27" s="1">
+      <c r="J27" s="3">
+        <v>1</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0</v>
+      </c>
+      <c r="L27" s="3">
         <v>0.99399999999999999</v>
       </c>
-      <c r="M27" s="1">
+      <c r="M27" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>